<commit_message>
Updated Pygad with results
</commit_message>
<xml_diff>
--- a/Optimization/Mathematical calculations (cost, intrest, linear stuff energy demand).xlsx
+++ b/Optimization/Mathematical calculations (cost, intrest, linear stuff energy demand).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jocke\Documents\Master-Thesis-Python-Coding\Optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF3F295-C770-4398-A2C3-2833C82EB0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606F18BE-BBB1-4244-93AA-E769123420B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="S25">
-        <f t="shared" ref="S25:S36" si="0">S24+1</f>
+        <f t="shared" ref="S25:S34" si="0">S24+1</f>
         <v>2011</v>
       </c>
       <c r="T25">

</xml_diff>

<commit_message>
All results and combined
</commit_message>
<xml_diff>
--- a/Optimization/Mathematical calculations (cost, intrest, linear stuff energy demand).xlsx
+++ b/Optimization/Mathematical calculations (cost, intrest, linear stuff energy demand).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jocke\Documents\Master-Thesis-Python-Coding\Optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606F18BE-BBB1-4244-93AA-E769123420B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBD3606-2F23-422F-9265-C09ADA837C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7050" yWindow="1200" windowWidth="19995" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
   <si>
     <t>Year</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>Capital cost capacity kWh</t>
-  </si>
-  <si>
     <t>Cost 2022 Euro</t>
   </si>
   <si>
@@ -244,6 +241,36 @@
   </si>
   <si>
     <t>Value pound</t>
+  </si>
+  <si>
+    <t>Storage Block $/kWh</t>
+  </si>
+  <si>
+    <t>Storage Balance of System $/kWh</t>
+  </si>
+  <si>
+    <t>Engineering, Procurement, and Construction $/kWh</t>
+  </si>
+  <si>
+    <t>Project Development $/kWh</t>
+  </si>
+  <si>
+    <t>Power Equipment $/kW</t>
+  </si>
+  <si>
+    <t>Controls &amp; Communication $/kW</t>
+  </si>
+  <si>
+    <t>Grid Integration $/kW</t>
+  </si>
+  <si>
+    <t>System Integration $/kWh</t>
+  </si>
+  <si>
+    <t>Capital cost capacity total kWh</t>
+  </si>
+  <si>
+    <t>Capital cost power total  kW</t>
   </si>
 </sst>
 </file>
@@ -287,7 +314,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +345,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -332,7 +365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -344,6 +377,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -943,7 +977,7 @@
         <v>17</v>
       </c>
       <c r="N23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
@@ -1318,7 +1352,7 @@
         <v>16</v>
       </c>
       <c r="M44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N44">
         <f>N42*100/O42</f>
@@ -1334,13 +1368,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201B5F2F-1C4B-4BDB-B0EE-557EB48B8CC1}">
   <dimension ref="B1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
@@ -1359,18 +1393,18 @@
   <sheetData>
     <row r="1" spans="2:25" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
         <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.25">
@@ -1390,17 +1424,17 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
         <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L3" t="s">
         <v>24</v>
@@ -1412,54 +1446,54 @@
         <v>0</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="X3" t="s">
         <v>32</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="C4">
-        <v>448</v>
+        <v>182</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4">
         <v>2020</v>
       </c>
       <c r="G4">
-        <f>C4/1.1218</f>
-        <v>399.35817436263153</v>
+        <f t="shared" ref="G4:G11" si="0">C4/1.1218</f>
+        <v>162.23925833481906</v>
       </c>
       <c r="H4" s="6">
         <f>G4*$U$17</f>
-        <v>427.31324656801576</v>
+        <v>173.59600641825639</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4">
         <v>221</v>
       </c>
       <c r="L4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" t="s">
         <v>58</v>
-      </c>
-      <c r="M4" t="s">
-        <v>59</v>
       </c>
       <c r="N4">
         <v>2009</v>
@@ -1469,51 +1503,51 @@
         <v>331.18873239436624</v>
       </c>
       <c r="S4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T4">
         <v>1</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C5">
-        <v>1793</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5">
         <v>2020</v>
       </c>
       <c r="G5">
-        <f>C5/1.1218</f>
-        <v>1598.3241219468712</v>
+        <f t="shared" si="0"/>
+        <v>37.439828846496702</v>
       </c>
       <c r="H5" s="6">
         <f>G5*$U$17</f>
-        <v>1710.2068104831524</v>
+        <v>40.060616865751477</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" t="s">
         <v>58</v>
-      </c>
-      <c r="M5" t="s">
-        <v>59</v>
       </c>
       <c r="N5">
         <v>2009</v>
@@ -1523,7 +1557,7 @@
         <v>1.4985915492957749</v>
       </c>
       <c r="S5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T5">
         <v>1.2134</v>
@@ -1531,31 +1565,31 @@
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C6">
-        <v>4.4000000000000004</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6">
         <v>2020</v>
       </c>
       <c r="G6">
-        <f>C6/1.1218</f>
-        <v>3.9222677839187026</v>
+        <f t="shared" si="0"/>
+        <v>44.571224817257985</v>
       </c>
       <c r="H6" s="6">
         <f>G6*$U$17</f>
-        <v>4.1968265287930118</v>
+        <v>47.691210554466046</v>
       </c>
       <c r="I6" s="1"/>
       <c r="S6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T6">
         <v>0.88749999999999996</v>
@@ -1563,61 +1597,201 @@
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C7">
-        <v>0.51249999999999996</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7">
         <v>2020</v>
       </c>
       <c r="G7">
-        <f>C7/1.1218</f>
-        <v>0.45685505437689428</v>
+        <f t="shared" si="0"/>
+        <v>54.376894277054738</v>
       </c>
       <c r="H7" s="6">
         <f>G7*$U$17</f>
-        <v>0.48883490818327691</v>
+        <v>58.183276876448573</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8">
+        <v>2020</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>65.073988233196658</v>
+      </c>
+      <c r="H8" s="6">
+        <f>G8*$U$17</f>
+        <v>69.629167409520434</v>
+      </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9">
+        <v>2020</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>75.771082189338571</v>
+      </c>
+      <c r="H9" s="6">
+        <f>G9*$U$17</f>
+        <v>81.075057942592281</v>
+      </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10">
+        <v>2020</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>35.656979853806384</v>
+      </c>
+      <c r="H10" s="6">
+        <f>G10*$U$17</f>
+        <v>38.152968443572831</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="T10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11">
+        <v>2020</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>27.634159386699949</v>
+      </c>
+      <c r="H11" s="6">
+        <f>G11*$U$17</f>
+        <v>29.568550543768946</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="T11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12">
+        <f>C4+C5+C6+C7+C8</f>
+        <v>408</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12">
+        <v>2020</v>
+      </c>
+      <c r="G12">
+        <f>C12/1.1218</f>
+        <v>363.70119450882515</v>
+      </c>
+      <c r="H12" s="7">
+        <f>G12*$U$17</f>
+        <v>389.16027812444293</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="S12" t="s">
         <v>18</v>
       </c>
       <c r="T12" t="s">
+        <v>54</v>
+      </c>
+      <c r="U12" t="s">
         <v>55</v>
       </c>
-      <c r="U12" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13">
+        <f>C9+C10+C11</f>
+        <v>156</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13">
+        <v>2020</v>
+      </c>
+      <c r="G13">
+        <f>C13/1.1218</f>
+        <v>139.0622214298449</v>
+      </c>
+      <c r="H13" s="7">
+        <f>G13*$U$17</f>
+        <v>148.79657692993405</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="S13">
         <v>2016</v>
@@ -1630,6 +1804,29 @@
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14">
+        <v>2020</v>
+      </c>
+      <c r="G14">
+        <f>C14/1.1218</f>
+        <v>3.9222677839187026</v>
+      </c>
+      <c r="H14" s="6">
+        <f>G14*$U$17</f>
+        <v>4.1968265287930118</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="S14">
         <v>2017</v>
@@ -1642,6 +1839,29 @@
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15">
+        <v>0.51249999999999996</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15">
+        <v>2020</v>
+      </c>
+      <c r="G15">
+        <f>C15/1.1218</f>
+        <v>0.45685505437689428</v>
+      </c>
+      <c r="H15" s="6">
+        <f>G15*$U$17</f>
+        <v>0.48883490818327691</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="S15">
         <v>2018</v>
@@ -1692,19 +1912,19 @@
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
       <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
         <v>28</v>
       </c>
-      <c r="E18" t="s">
-        <v>29</v>
-      </c>
       <c r="F18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" t="s">
         <v>22</v>
@@ -1721,10 +1941,10 @@
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
         <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
       </c>
       <c r="D19">
         <v>2017</v>
@@ -1733,18 +1953,18 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" t="s">
         <v>41</v>
-      </c>
-      <c r="H19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="T21" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
@@ -1752,10 +1972,10 @@
         <v>18</v>
       </c>
       <c r="T22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
@@ -1783,7 +2003,7 @@
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="S25">
-        <f t="shared" ref="S25:S34" si="0">S24+1</f>
+        <f t="shared" ref="S25:S34" si="1">S24+1</f>
         <v>2011</v>
       </c>
       <c r="T25">
@@ -1795,7 +2015,7 @@
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="S26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2012</v>
       </c>
       <c r="T26">
@@ -1807,7 +2027,7 @@
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="S27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2013</v>
       </c>
       <c r="T27">
@@ -1819,7 +2039,7 @@
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="S28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2014</v>
       </c>
       <c r="T28">
@@ -1831,7 +2051,7 @@
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="S29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2015</v>
       </c>
       <c r="T29">
@@ -1843,7 +2063,7 @@
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="S30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2016</v>
       </c>
       <c r="T30">
@@ -1855,7 +2075,7 @@
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="S31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2017</v>
       </c>
       <c r="T31">
@@ -1867,7 +2087,7 @@
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="S32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2018</v>
       </c>
       <c r="T32">
@@ -1891,7 +2111,7 @@
     </row>
     <row r="34" spans="19:21" x14ac:dyDescent="0.25">
       <c r="S34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2020</v>
       </c>
       <c r="T34">

</xml_diff>